<commit_message>
Atualizando formatacao das rodadas escolhidas no 4-4-2 da base completa
</commit_message>
<xml_diff>
--- a/analises_dos_dados_preliminares/4-4-2 -----Times mais caros por rodada X Times Escolhidos Pelo algoritmos-----Base Completa.xlsx
+++ b/analises_dos_dados_preliminares/4-4-2 -----Times mais caros por rodada X Times Escolhidos Pelo algoritmos-----Base Completa.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dpcrj\OneDrive\Área de Trabalho\Faculdade\TCC_code\sportsAnalytics\analises_dos_dados_preliminares\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{125E2907-71D8-4213-94BF-92BED47B2F3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C450AD3-450E-4B20-BF9E-3789C9D2A6DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="3" activeTab="9" xr2:uid="{FCE826C4-9F25-4A22-BADC-C872D1D1AAC8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{FCE826C4-9F25-4A22-BADC-C872D1D1AAC8}"/>
   </bookViews>
   <sheets>
     <sheet name="rodada 01" sheetId="40" r:id="rId1"/>
@@ -435,9 +435,6 @@
     <t>Eduardo Luís Abonizio de Souza</t>
   </si>
   <si>
-    <t>Time escalado com 88,85 cartoletas pq ao final da rodada 7 tinhamos disponiveis 89.72999999999995 Cartoletas</t>
-  </si>
-  <si>
     <t>Luiz Felipe do Nascimento dos Santos</t>
   </si>
   <si>
@@ -475,13 +472,16 @@
   </si>
   <si>
     <t>Time escalado com 82,77 cartoletas pq ao final da rodada 9 tinhamos disponiveis 83,00999999999996 Cartoletas</t>
+  </si>
+  <si>
+    <t>Time escalado com 88,85 cartoletas pq ao final da rodada 7 tinhamos disponiveis 89,72999999999995 Cartoletas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -500,6 +500,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B0F0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -534,7 +541,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -557,14 +564,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -882,8 +895,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A61E21B-ABB0-49B8-8EC3-6C08DA64520D}">
   <dimension ref="A1:AC16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -945,7 +958,7 @@
       </c>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="10" t="s">
         <v>42</v>
       </c>
       <c r="B2" s="1">
@@ -1033,7 +1046,7 @@
       </c>
     </row>
     <row r="4" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="10" t="s">
         <v>34</v>
       </c>
       <c r="B4" s="1">
@@ -1385,7 +1398,7 @@
       </c>
     </row>
     <row r="12" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="10" t="s">
         <v>51</v>
       </c>
       <c r="B12" s="1">
@@ -1508,8 +1521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B526A04-573F-43AA-A380-3041667B0AA3}">
   <dimension ref="A1:AC20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26:G37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1609,7 +1622,7 @@
     </row>
     <row r="3" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B3" s="1">
         <v>69138</v>
@@ -1624,7 +1637,7 @@
         <v>10.199999999999999</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G3" s="2">
         <v>92146</v>
@@ -1660,7 +1673,7 @@
         <v>7.96</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G4" s="2">
         <v>38509</v>
@@ -1696,7 +1709,7 @@
         <v>9.5</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G5" s="2">
         <v>104625</v>
@@ -1732,7 +1745,7 @@
         <v>9.4600000000000009</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G6" s="2">
         <v>95738</v>
@@ -1752,7 +1765,7 @@
       <c r="AC6" s="1"/>
     </row>
     <row r="7" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="9" t="s">
         <v>17</v>
       </c>
       <c r="B7" s="1">
@@ -1768,7 +1781,7 @@
         <v>12.62</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G7" s="2">
         <v>73501</v>
@@ -1804,7 +1817,7 @@
         <v>6.93</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G8" s="2">
         <v>83004</v>
@@ -1824,8 +1837,8 @@
       <c r="AC8" s="1"/>
     </row>
     <row r="9" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
-        <v>136</v>
+      <c r="A9" s="9" t="s">
+        <v>135</v>
       </c>
       <c r="B9" s="1">
         <v>83004</v>
@@ -1896,8 +1909,8 @@
       <c r="AC10" s="1"/>
     </row>
     <row r="11" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
-        <v>137</v>
+      <c r="A11" s="9" t="s">
+        <v>136</v>
       </c>
       <c r="B11" s="1">
         <v>71224</v>
@@ -1912,7 +1925,7 @@
         <v>9.75</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G11" s="2">
         <v>71224</v>
@@ -1932,7 +1945,7 @@
       <c r="AC11" s="1"/>
     </row>
     <row r="12" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="9" t="s">
         <v>112</v>
       </c>
       <c r="B12" s="1">
@@ -1948,7 +1961,7 @@
         <v>6.94</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G12" s="2">
         <v>89226</v>
@@ -1969,7 +1982,7 @@
     </row>
     <row r="13" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B13" s="1">
         <v>79035</v>
@@ -2029,13 +2042,13 @@
     <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="C16" s="4"/>
     </row>
-    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F17" s="8" t="s">
-        <v>143</v>
+    <row r="17" spans="6:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="F17" s="12" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="20" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F20" s="9"/>
+      <c r="F20" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -2048,7 +2061,7 @@
   <dimension ref="A1:AC17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2146,7 +2159,7 @@
       <c r="AC2" s="1"/>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="10" t="s">
         <v>60</v>
       </c>
       <c r="B3" s="1">
@@ -2326,7 +2339,7 @@
       <c r="AC7" s="1"/>
     </row>
     <row r="8" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="10" t="s">
         <v>61</v>
       </c>
       <c r="B8" s="1">
@@ -2398,7 +2411,7 @@
       <c r="AC9" s="1"/>
     </row>
     <row r="10" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="10" t="s">
         <v>62</v>
       </c>
       <c r="B10" s="1">
@@ -2470,7 +2483,7 @@
       <c r="AC11" s="1"/>
     </row>
     <row r="12" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="10" t="s">
         <v>63</v>
       </c>
       <c r="B12" s="1">
@@ -2567,8 +2580,8 @@
     <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="C16" s="4"/>
     </row>
-    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F17" s="8" t="s">
+    <row r="17" spans="6:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="F17" s="12" t="s">
         <v>89</v>
       </c>
     </row>
@@ -2583,7 +2596,7 @@
   <dimension ref="A1:AC36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2645,7 +2658,7 @@
       </c>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1">
@@ -2681,7 +2694,7 @@
       <c r="AC2" s="1"/>
     </row>
     <row r="3" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="10" t="s">
         <v>71</v>
       </c>
       <c r="B3" s="1">
@@ -2789,7 +2802,7 @@
       <c r="AC5" s="1"/>
     </row>
     <row r="6" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="10" t="s">
         <v>73</v>
       </c>
       <c r="B6" s="1">
@@ -2825,7 +2838,7 @@
       <c r="AC6" s="1"/>
     </row>
     <row r="7" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="10" t="s">
         <v>61</v>
       </c>
       <c r="B7" s="1">
@@ -2897,7 +2910,7 @@
       <c r="AC8" s="1"/>
     </row>
     <row r="9" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="10" t="s">
         <v>75</v>
       </c>
       <c r="B9" s="1">
@@ -2933,7 +2946,7 @@
       <c r="AC9" s="1"/>
     </row>
     <row r="10" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="10" t="s">
         <v>76</v>
       </c>
       <c r="B10" s="1">
@@ -2969,7 +2982,7 @@
       <c r="AC10" s="1"/>
     </row>
     <row r="11" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="10" t="s">
         <v>77</v>
       </c>
       <c r="B11" s="1">
@@ -3005,7 +3018,7 @@
       <c r="AC11" s="1"/>
     </row>
     <row r="12" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="10" t="s">
         <v>78</v>
       </c>
       <c r="B12" s="1">
@@ -3102,13 +3115,13 @@
     <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="C16" s="4"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F17" s="8" t="s">
+    <row r="17" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="F17" s="12" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F20" s="9"/>
+      <c r="F20" s="8"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
@@ -3181,7 +3194,7 @@
   <dimension ref="A1:AC20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" activeCellId="4" sqref="A2 A3 A5 A13 A7"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3244,7 +3257,7 @@
       </c>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="9" t="s">
         <v>82</v>
       </c>
       <c r="B2" s="1">
@@ -3280,7 +3293,7 @@
       <c r="AC2" s="1"/>
     </row>
     <row r="3" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="9" t="s">
         <v>83</v>
       </c>
       <c r="B3" s="1">
@@ -3352,7 +3365,7 @@
       <c r="AC4" s="1"/>
     </row>
     <row r="5" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="9" t="s">
         <v>84</v>
       </c>
       <c r="B5" s="1">
@@ -3424,7 +3437,7 @@
       <c r="AC6" s="1"/>
     </row>
     <row r="7" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="9" t="s">
         <v>85</v>
       </c>
       <c r="B7" s="1">
@@ -3640,7 +3653,7 @@
       <c r="AC12" s="1"/>
     </row>
     <row r="13" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
+      <c r="A13" s="9" t="s">
         <v>87</v>
       </c>
       <c r="B13" s="1">
@@ -3701,13 +3714,13 @@
     <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="C16" s="4"/>
     </row>
-    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F17" s="8" t="s">
+    <row r="17" spans="6:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="F17" s="12" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="20" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F20" s="9"/>
+      <c r="F20" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -3720,7 +3733,7 @@
   <dimension ref="A1:AC20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3783,7 +3796,7 @@
       </c>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="9" t="s">
         <v>95</v>
       </c>
       <c r="B2" s="1">
@@ -3819,7 +3832,7 @@
       <c r="AC2" s="1"/>
     </row>
     <row r="3" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="9" t="s">
         <v>96</v>
       </c>
       <c r="B3" s="1">
@@ -3891,7 +3904,7 @@
       <c r="AC4" s="1"/>
     </row>
     <row r="5" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="9" t="s">
         <v>15</v>
       </c>
       <c r="B5" s="1">
@@ -3963,7 +3976,7 @@
       <c r="AC6" s="1"/>
     </row>
     <row r="7" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="9" t="s">
         <v>97</v>
       </c>
       <c r="B7" s="1">
@@ -3999,7 +4012,7 @@
       <c r="AC7" s="1"/>
     </row>
     <row r="8" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="9" t="s">
         <v>98</v>
       </c>
       <c r="B8" s="1">
@@ -4035,7 +4048,7 @@
       <c r="AC8" s="1"/>
     </row>
     <row r="9" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="9" t="s">
         <v>85</v>
       </c>
       <c r="B9" s="1">
@@ -4240,13 +4253,13 @@
     <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="C16" s="4"/>
     </row>
-    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F17" s="8" t="s">
+    <row r="17" spans="6:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="F17" s="12" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="20" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F20" s="9"/>
+      <c r="F20" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -4259,7 +4272,7 @@
   <dimension ref="A1:AC20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4430,7 +4443,7 @@
       <c r="AC4" s="1"/>
     </row>
     <row r="5" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="9" t="s">
         <v>107</v>
       </c>
       <c r="B5" s="1">
@@ -4466,7 +4479,7 @@
       <c r="AC5" s="1"/>
     </row>
     <row r="6" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="9" t="s">
         <v>108</v>
       </c>
       <c r="B6" s="1">
@@ -4502,7 +4515,7 @@
       <c r="AC6" s="1"/>
     </row>
     <row r="7" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="9" t="s">
         <v>85</v>
       </c>
       <c r="B7" s="1">
@@ -4682,7 +4695,7 @@
       <c r="AC11" s="1"/>
     </row>
     <row r="12" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="9" t="s">
         <v>111</v>
       </c>
       <c r="B12" s="1">
@@ -4718,7 +4731,7 @@
       <c r="AC12" s="1"/>
     </row>
     <row r="13" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
+      <c r="A13" s="9" t="s">
         <v>112</v>
       </c>
       <c r="B13" s="1">
@@ -4779,13 +4792,13 @@
     <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="C16" s="4"/>
     </row>
-    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F17" s="8" t="s">
+    <row r="17" spans="6:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="F17" s="12" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="20" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F20" s="9"/>
+      <c r="F20" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -4798,7 +4811,7 @@
   <dimension ref="A1:AC20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4933,7 +4946,7 @@
       <c r="AC3" s="1"/>
     </row>
     <row r="4" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="9" t="s">
         <v>118</v>
       </c>
       <c r="B4" s="1">
@@ -4969,7 +4982,7 @@
       <c r="AC4" s="1"/>
     </row>
     <row r="5" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="9" t="s">
         <v>107</v>
       </c>
       <c r="B5" s="1">
@@ -5041,7 +5054,7 @@
       <c r="AC6" s="1"/>
     </row>
     <row r="7" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="9" t="s">
         <v>85</v>
       </c>
       <c r="B7" s="1">
@@ -5185,7 +5198,7 @@
       <c r="AC10" s="1"/>
     </row>
     <row r="11" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="9" t="s">
         <v>119</v>
       </c>
       <c r="B11" s="1">
@@ -5221,7 +5234,7 @@
       <c r="AC11" s="1"/>
     </row>
     <row r="12" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="9" t="s">
         <v>112</v>
       </c>
       <c r="B12" s="1">
@@ -5318,13 +5331,13 @@
     <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="C16" s="4"/>
     </row>
-    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F17" s="8" t="s">
+    <row r="17" spans="6:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="F17" s="12" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="20" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F20" s="9"/>
+      <c r="F20" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -5337,7 +5350,7 @@
   <dimension ref="A1:AC20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5472,7 +5485,7 @@
       <c r="AC3" s="1"/>
     </row>
     <row r="4" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="9" t="s">
         <v>125</v>
       </c>
       <c r="B4" s="1">
@@ -5580,7 +5593,7 @@
       <c r="AC6" s="1"/>
     </row>
     <row r="7" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="9" t="s">
         <v>126</v>
       </c>
       <c r="B7" s="1">
@@ -5616,7 +5629,7 @@
       <c r="AC7" s="1"/>
     </row>
     <row r="8" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="9" t="s">
         <v>127</v>
       </c>
       <c r="B8" s="1">
@@ -5652,7 +5665,7 @@
       <c r="AC8" s="1"/>
     </row>
     <row r="9" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="9" t="s">
         <v>85</v>
       </c>
       <c r="B9" s="1">
@@ -5724,7 +5737,7 @@
       <c r="AC10" s="1"/>
     </row>
     <row r="11" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="9" t="s">
         <v>119</v>
       </c>
       <c r="B11" s="1">
@@ -5796,7 +5809,7 @@
       <c r="AC12" s="1"/>
     </row>
     <row r="13" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
+      <c r="A13" s="9" t="s">
         <v>112</v>
       </c>
       <c r="B13" s="1">
@@ -5857,13 +5870,13 @@
     <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="C16" s="4"/>
     </row>
-    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F17" s="8" t="s">
-        <v>130</v>
+    <row r="17" spans="6:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="F17" s="11" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="20" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F20" s="9"/>
+      <c r="F20" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -5876,7 +5889,7 @@
   <dimension ref="A1:AC37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5939,7 +5952,7 @@
       </c>
     </row>
     <row r="2" spans="1:29" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="9" t="s">
         <v>128</v>
       </c>
       <c r="B2" s="1">
@@ -6011,7 +6024,7 @@
       <c r="AC3" s="1"/>
     </row>
     <row r="4" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="9" t="s">
         <v>125</v>
       </c>
       <c r="B4" s="1">
@@ -6047,7 +6060,7 @@
       <c r="AC4" s="1"/>
     </row>
     <row r="5" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="9" t="s">
         <v>107</v>
       </c>
       <c r="B5" s="1">
@@ -6063,7 +6076,7 @@
         <v>11.55</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G5" s="2">
         <v>104257</v>
@@ -6119,7 +6132,7 @@
       <c r="AC6" s="1"/>
     </row>
     <row r="7" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="9" t="s">
         <v>85</v>
       </c>
       <c r="B7" s="1">
@@ -6171,7 +6184,7 @@
         <v>6.28</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G8" s="2">
         <v>73501</v>
@@ -6299,7 +6312,7 @@
       <c r="AC11" s="1"/>
     </row>
     <row r="12" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="9" t="s">
         <v>112</v>
       </c>
       <c r="B12" s="1">
@@ -6315,7 +6328,7 @@
         <v>7.8</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G12" s="2">
         <v>79035</v>
@@ -6335,8 +6348,8 @@
       <c r="AC12" s="1"/>
     </row>
     <row r="13" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
-        <v>131</v>
+      <c r="A13" s="9" t="s">
+        <v>130</v>
       </c>
       <c r="B13" s="1">
         <v>79035</v>
@@ -6396,13 +6409,13 @@
     <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="C16" s="4"/>
     </row>
-    <row r="17" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F17" s="8" t="s">
-        <v>134</v>
+    <row r="17" spans="6:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="F17" s="12" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="20" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F20" s="9"/>
+      <c r="F20" s="8"/>
     </row>
     <row r="26" spans="6:7" x14ac:dyDescent="0.25">
       <c r="G26" s="2">

</xml_diff>

<commit_message>
Adicionanado arquivos csv com os times de maiores scores por esquema tático e tabela resumo.
</commit_message>
<xml_diff>
--- a/analises_dos_dados_preliminares/4-4-2 -----Times mais caros por rodada X Times Escolhidos Pelo algoritmos-----Base Completa.xlsx
+++ b/analises_dos_dados_preliminares/4-4-2 -----Times mais caros por rodada X Times Escolhidos Pelo algoritmos-----Base Completa.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dpcrj\OneDrive\Área de Trabalho\Faculdade\TCC_code\sportsAnalytics\analises_dos_dados_preliminares\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C450AD3-450E-4B20-BF9E-3789C9D2A6DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27B94F38-7A65-48CA-95C1-2E404A785EB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{FCE826C4-9F25-4A22-BADC-C872D1D1AAC8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="3" activeTab="9" xr2:uid="{FCE826C4-9F25-4A22-BADC-C872D1D1AAC8}"/>
   </bookViews>
   <sheets>
     <sheet name="rodada 01" sheetId="40" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="148">
   <si>
     <t>Everaldo Stum</t>
   </si>
@@ -475,6 +475,18 @@
   </si>
   <si>
     <t>Time escalado com 88,85 cartoletas pq ao final da rodada 7 tinhamos disponiveis 89,72999999999995 Cartoletas</t>
+  </si>
+  <si>
+    <t>pegar melhor escalacao possivel por rodada</t>
+  </si>
+  <si>
+    <t>qual esquema deu maior pontuacao</t>
+  </si>
+  <si>
+    <t>no final das 38 rodadas melhor possivel de cada escalação a cada rodada e soma</t>
+  </si>
+  <si>
+    <t>somando somente o valor de score</t>
   </si>
 </sst>
 </file>
@@ -541,7 +553,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -578,6 +590,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -895,7 +910,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A61E21B-ABB0-49B8-8EC3-6C08DA64520D}">
   <dimension ref="A1:AC16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
@@ -1519,10 +1534,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B526A04-573F-43AA-A380-3041667B0AA3}">
-  <dimension ref="A1:AC20"/>
+  <dimension ref="A1:AC22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:XFD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2042,13 +2057,31 @@
     <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="C16" s="4"/>
     </row>
-    <row r="17" spans="6:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="F17" s="12" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="20" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="13" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="13" t="s">
+        <v>145</v>
+      </c>
       <c r="F20" s="8"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="13" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>147</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -5889,7 +5922,7 @@
   <dimension ref="A1:AC37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>